<commit_message>
added all station and pokayoke automail  concept established
</commit_message>
<xml_diff>
--- a/templates/Excel/ST1_POKA-YOKE.xlsx
+++ b/templates/Excel/ST1_POKA-YOKE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,19 +642,706 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>489</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>54</t>
+      <c r="M3" t="n">
+        <v>489</v>
+      </c>
+      <c r="N3" t="n">
+        <v>45</v>
+      </c>
+      <c r="O3" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-02-10T11:25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-02-10T11:25</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-02-10T11:57</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Mail</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>SuriyaPRAKASH</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>PRAKASH</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-02-10T11:59</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>MAIL</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>TESTIN</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>TESINT</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-02-10T12:16</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>85*</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>418</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-02-10T14:25</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Mail</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-02-10T14:32</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Mail</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-02-10T16:44</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Suriya</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Suriya</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-02-11T11:35</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SHIFT1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>testing</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>testing</t>
         </is>
       </c>
     </row>

</xml_diff>